<commit_message>
prepared for simulator B testing 4
</commit_message>
<xml_diff>
--- a/src/data/variables_data_documentation.xlsx
+++ b/src/data/variables_data_documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Documents\05_Kurse_und_Fortbildung\WUR_Autonomous_Greenhouse_Challenge_4th_Edition\marcel-code\smart_tomAItoes_simulation\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363923CF-CFC7-4BEF-A762-E8C6AFF2FB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91FC65B-A0B5-4543-A860-A814DA2AE7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_variables" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="104">
   <si>
     <t>Folder</t>
   </si>
@@ -313,6 +313,33 @@
   </si>
   <si>
     <t>Possible Datatype/s</t>
+  </si>
+  <si>
+    <t>20240507_simulator_B_generated</t>
+  </si>
+  <si>
+    <t>20240520_simulator_A_generated</t>
+  </si>
+  <si>
+    <t>20240521_simulator_B_generated</t>
+  </si>
+  <si>
+    <t>20240522_simulator_A_generated</t>
+  </si>
+  <si>
+    <t>4th intervall for simulator A</t>
+  </si>
+  <si>
+    <t>5th intervall for simulator A</t>
+  </si>
+  <si>
+    <t>3rd time</t>
+  </si>
+  <si>
+    <t>4th time</t>
+  </si>
+  <si>
+    <t>tested different parameter combinations with = data generation. Kept constant simulation interval.</t>
   </si>
 </sst>
 </file>
@@ -4378,7 +4405,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4894,10 +4921,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5011,12 +5038,96 @@
         <v>17</v>
       </c>
     </row>
+    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5">
+        <v>45419</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5">
+        <v>45432</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5">
+        <v>45433</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5">
+        <v>45434</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" location="initial_parameter_values!A1" display="initial_parameters" xr:uid="{B627225B-7216-40D4-9EF6-18F7EB55723D}"/>
     <hyperlink ref="F3" location="initial_parameter_values!A1" display="initial_parameters" xr:uid="{A5621A63-9696-4D41-B100-F60657B021EB}"/>
     <hyperlink ref="F4" location="initial_parameter_values!A1" display="initial_parameters" xr:uid="{8822E33A-646A-41FD-9A1E-360D9F7F213D}"/>
     <hyperlink ref="F5" location="initial_parameter_values!A1" display="initial_parameters" xr:uid="{D669A377-DE89-44CC-9A6A-3E9A2FCD2064}"/>
+    <hyperlink ref="F6" location="initial_parameter_values!A1" display="initial_parameters" xr:uid="{A4025172-79E4-457F-B662-FAA62D1731AB}"/>
+    <hyperlink ref="F7" location="initial_parameter_values!A1" display="initial_parameters" xr:uid="{DB3E1173-4CEC-47D3-BD75-785253AB206B}"/>
+    <hyperlink ref="F8" location="initial_parameter_values!A1" display="initial_parameters" xr:uid="{9915FA4C-BF3C-491F-97E6-D500AC0435B0}"/>
+    <hyperlink ref="F9" location="initial_parameter_values!A1" display="initial_parameters" xr:uid="{CE031774-11DA-4E69-938C-97E08CBB32A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>